<commit_message>
push articles and schedule
</commit_message>
<xml_diff>
--- a/PSY-GS-8875_Course_Schedule_S2024.xlsx
+++ b/PSY-GS-8875_Course_Schedule_S2024.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="139">
   <si>
     <t xml:space="preserve">Week</t>
   </si>
@@ -57,7 +57,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">“Understanding” section: </t>
+      <t xml:space="preserve">“Understanding” section </t>
     </r>
     <r>
       <rPr>
@@ -128,7 +128,7 @@
     <t xml:space="preserve">ridge (l2-norm) regression</t>
   </si>
   <si>
-    <t xml:space="preserve">screening for math success</t>
+    <t xml:space="preserve">predicting life outcomes with personality</t>
   </si>
   <si>
     <t xml:space="preserve">ESL Chapters 3.4, 3.4.1, 3.4.2, and 4.4.4</t>
@@ -254,54 +254,57 @@
     <t xml:space="preserve">ESL Chapters: 17.1-17.3</t>
   </si>
   <si>
+    <t xml:space="preserve">application will be limited to in-class ma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schmittmann et al. - 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">network estimation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EBICglasso: Epskamp &amp; Fried – 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Louvain: Blondel et al. - 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">community detection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Walktrap: Pons and Latapy - 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Many different algorithms: Christensen et al. - 2023 – community</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exploratory graph analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EGA: Golino &amp; Epskamp – 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EGA with TMFG: Golino et al. - 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unidimensionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unidimensionality: Christensen – 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bootstrap exploratory graph analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extraversion by country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christensen &amp; Golino – 2021 – bootEGA</t>
+  </si>
+  <si>
     <t xml:space="preserve">application will be limited to in-class materials</t>
   </si>
   <si>
-    <t xml:space="preserve">Schmittmann et al. - 2013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">network estimation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EBICglasso: Epskamp &amp; Fried – 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Louvain: Blondel et al. - 2008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">community detection</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Walktrap: Pons and Latapy - 2006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Many different algorithms: Christensen et al. - 2023 – community</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exploratory graph analysis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EGA: Golino &amp; Epskamp – 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EGA with TMFG: Golino et al. - 2020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unidimensionality</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christensen – 2024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bootstrap exploratory graph analysis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">extraversion by country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Christensen &amp; Golino – 2021 – bootEGA</t>
-  </si>
-  <si>
     <t xml:space="preserve">Personality taxonomy: Samo et al. - 2023</t>
   </si>
   <si>
@@ -377,6 +380,9 @@
     <t xml:space="preserve">initial check for survey item local dependence and IRT linking</t>
   </si>
   <si>
+    <t xml:space="preserve">Attention: Vaswani et al. - 2017</t>
+  </si>
+  <si>
     <t xml:space="preserve">NLP: Chapters 1-3 and 5</t>
   </si>
   <si>
@@ -384,6 +390,9 @@
   </si>
   <si>
     <t xml:space="preserve">sentence similarity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Formal algorithms: Phuong and Hutter - 2022</t>
   </si>
   <si>
     <t xml:space="preserve">Automatic item generation: Hommel et al. - 2021</t>
@@ -754,7 +763,7 @@
   <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="28.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -819,7 +828,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="7"/>
-      <c r="E3" s="9"/>
+      <c r="E3" s="7"/>
       <c r="F3" s="9"/>
       <c r="G3" s="7"/>
     </row>
@@ -830,8 +839,8 @@
         <v>12</v>
       </c>
       <c r="D4" s="7"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
       <c r="G4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -934,7 +943,7 @@
       <c r="C11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="11" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="11" t="s">
@@ -953,9 +962,9 @@
       <c r="C12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
       <c r="G12" s="2" t="s">
         <v>34</v>
       </c>
@@ -1204,21 +1213,21 @@
         <v>80</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="7" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="7" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
@@ -1227,11 +1236,11 @@
       <c r="A29" s="7"/>
       <c r="B29" s="8"/>
       <c r="C29" s="7" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="7" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
@@ -1240,11 +1249,11 @@
       <c r="A30" s="7"/>
       <c r="B30" s="8"/>
       <c r="C30" s="7" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
@@ -1253,22 +1262,22 @@
       <c r="A31" s="7"/>
       <c r="B31" s="8"/>
       <c r="C31" s="7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
     </row>
-    <row r="32" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
       <c r="B32" s="10" t="n">
         <v>45364</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="6"/>
@@ -1283,65 +1292,65 @@
         <v>45371</v>
       </c>
       <c r="C33" s="7" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="7"/>
       <c r="B34" s="8"/>
       <c r="C34" s="7" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="7" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="7"/>
       <c r="B35" s="8"/>
       <c r="C35" s="7" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="7" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="7"/>
       <c r="B36" s="8"/>
       <c r="C36" s="7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="n">
         <v>11</v>
       </c>
@@ -1349,7 +1358,7 @@
         <v>45378</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1363,50 +1372,52 @@
         <v>45385</v>
       </c>
       <c r="C38" s="7" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="7"/>
       <c r="B39" s="8"/>
       <c r="C39" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D39" s="9"/>
-      <c r="E39" s="7"/>
+      <c r="E39" s="7" t="s">
+        <v>111</v>
+      </c>
       <c r="F39" s="7"/>
       <c r="G39" s="7" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="43.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="7"/>
       <c r="B40" s="8"/>
       <c r="C40" s="7" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="7" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
         <v>13</v>
       </c>
@@ -1414,13 +1425,13 @@
         <v>45392</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="7" t="n">
         <v>14</v>
       </c>
@@ -1428,7 +1439,7 @@
         <v>45399</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
@@ -1457,7 +1468,7 @@
       <c r="B49" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="60">
+  <mergeCells count="62">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="D2:D4"/>
@@ -1512,11 +1523,13 @@
     <mergeCell ref="D33:D36"/>
     <mergeCell ref="F33:F36"/>
     <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C37:G37"/>
     <mergeCell ref="A38:A40"/>
     <mergeCell ref="B38:B40"/>
     <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E40"/>
     <mergeCell ref="F38:F40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C41:G41"/>
     <mergeCell ref="C42:G42"/>
   </mergeCells>
   <hyperlinks>
@@ -1541,7 +1554,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="43.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1555,86 +1568,86 @@
   <sheetData>
     <row r="1" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="15" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C3" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="43.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>